<commit_message>
Added reference_genome field for 1508samples
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.26.balsamic_qc.xlsx
+++ b/tests/fixtures/orderforms/1508.26.balsamic_qc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annick.renevey/Projects/cg/tests/fixtures/orderforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent.janvid/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEBD176-86E4-6649-B619-8328FE707A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D927E0-8144-CB4B-A94A-D726717D7D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35940" yWindow="-4500" windowWidth="28800" windowHeight="15520" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="705">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -5337,8 +5337,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -12995,7 +12995,7 @@
         <v>620</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E15" s="77" t="s">
         <v>663</v>
@@ -13035,18 +13035,12 @@
         <v>81</v>
       </c>
       <c r="R15" s="48"/>
-      <c r="S15" s="166" t="s">
-        <v>505</v>
-      </c>
+      <c r="S15" s="166"/>
       <c r="T15" s="120" t="s">
-        <v>79</v>
-      </c>
-      <c r="U15" s="75" t="s">
-        <v>579</v>
-      </c>
-      <c r="V15" s="75" t="s">
-        <v>580</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="U15" s="75"/>
+      <c r="V15" s="75"/>
       <c r="W15" s="82"/>
       <c r="X15" s="168"/>
       <c r="Y15" s="84"/>
@@ -14081,7 +14075,7 @@
         <v>620</v>
       </c>
       <c r="D16" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E16" s="77" t="s">
         <v>664</v>
@@ -14117,11 +14111,9 @@
       <c r="P16" s="81"/>
       <c r="Q16" s="97"/>
       <c r="R16" s="48"/>
-      <c r="S16" s="163" t="s">
-        <v>82</v>
-      </c>
+      <c r="S16" s="163"/>
       <c r="T16" s="120" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="U16" s="85"/>
       <c r="V16" s="86"/>
@@ -15147,7 +15139,7 @@
         <v>620</v>
       </c>
       <c r="D17" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E17" s="77" t="s">
         <v>665</v>
@@ -15156,7 +15148,7 @@
         <v>96</v>
       </c>
       <c r="G17" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H17" s="79" t="s">
         <v>76</v>
@@ -15183,9 +15175,7 @@
       <c r="P17" s="81"/>
       <c r="Q17" s="97"/>
       <c r="R17" s="48"/>
-      <c r="S17" s="163" t="s">
-        <v>94</v>
-      </c>
+      <c r="S17" s="163"/>
       <c r="T17" s="120" t="s">
         <v>97</v>
       </c>
@@ -16209,7 +16199,7 @@
         <v>620</v>
       </c>
       <c r="D18" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E18" s="77" t="s">
         <v>666</v>
@@ -16218,7 +16208,7 @@
         <v>124</v>
       </c>
       <c r="G18" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H18" s="79" t="s">
         <v>76</v>
@@ -16245,9 +16235,7 @@
       <c r="P18" s="81"/>
       <c r="Q18" s="97"/>
       <c r="R18" s="48"/>
-      <c r="S18" s="163" t="s">
-        <v>103</v>
-      </c>
+      <c r="S18" s="163"/>
       <c r="T18" s="120" t="s">
         <v>97</v>
       </c>
@@ -17271,7 +17259,7 @@
         <v>620</v>
       </c>
       <c r="D19" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E19" s="77" t="s">
         <v>667</v>
@@ -17280,7 +17268,7 @@
         <v>483</v>
       </c>
       <c r="G19" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H19" s="79" t="s">
         <v>76</v>
@@ -17307,9 +17295,7 @@
       <c r="P19" s="81"/>
       <c r="Q19" s="97"/>
       <c r="R19" s="48"/>
-      <c r="S19" s="163" t="s">
-        <v>109</v>
-      </c>
+      <c r="S19" s="163"/>
       <c r="T19" s="120" t="s">
         <v>97</v>
       </c>
@@ -18333,7 +18319,7 @@
         <v>620</v>
       </c>
       <c r="D20" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E20" s="77" t="s">
         <v>668</v>
@@ -18342,7 +18328,7 @@
         <v>503</v>
       </c>
       <c r="G20" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H20" s="79" t="s">
         <v>76</v>
@@ -18369,9 +18355,7 @@
       <c r="P20" s="81"/>
       <c r="Q20" s="97"/>
       <c r="R20" s="48"/>
-      <c r="S20" s="163" t="s">
-        <v>114</v>
-      </c>
+      <c r="S20" s="163"/>
       <c r="T20" s="120" t="s">
         <v>97</v>
       </c>
@@ -19395,7 +19379,7 @@
         <v>620</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E21" s="77" t="s">
         <v>669</v>
@@ -19404,7 +19388,7 @@
         <v>484</v>
       </c>
       <c r="G21" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H21" s="79" t="s">
         <v>76</v>
@@ -19431,9 +19415,7 @@
       <c r="P21" s="81"/>
       <c r="Q21" s="97"/>
       <c r="R21" s="48"/>
-      <c r="S21" s="163" t="s">
-        <v>118</v>
-      </c>
+      <c r="S21" s="163"/>
       <c r="T21" s="120" t="s">
         <v>97</v>
       </c>
@@ -20457,7 +20439,7 @@
         <v>620</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E22" s="77" t="s">
         <v>670</v>
@@ -20466,7 +20448,7 @@
         <v>485</v>
       </c>
       <c r="G22" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H22" s="79" t="s">
         <v>76</v>
@@ -20493,9 +20475,7 @@
       <c r="P22" s="81"/>
       <c r="Q22" s="97"/>
       <c r="R22" s="48"/>
-      <c r="S22" s="163" t="s">
-        <v>123</v>
-      </c>
+      <c r="S22" s="163"/>
       <c r="T22" s="120" t="s">
         <v>97</v>
       </c>
@@ -21519,7 +21499,7 @@
         <v>620</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E23" s="77" t="s">
         <v>671</v>
@@ -21528,7 +21508,7 @@
         <v>486</v>
       </c>
       <c r="G23" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H23" s="79" t="s">
         <v>76</v>
@@ -21555,9 +21535,7 @@
       <c r="P23" s="81"/>
       <c r="Q23" s="97"/>
       <c r="R23" s="48"/>
-      <c r="S23" s="163" t="s">
-        <v>128</v>
-      </c>
+      <c r="S23" s="163"/>
       <c r="T23" s="120" t="s">
         <v>97</v>
       </c>
@@ -22581,7 +22559,7 @@
         <v>620</v>
       </c>
       <c r="D24" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E24" s="77" t="s">
         <v>672</v>
@@ -22590,7 +22568,7 @@
         <v>504</v>
       </c>
       <c r="G24" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H24" s="79" t="s">
         <v>76</v>
@@ -22617,9 +22595,7 @@
       <c r="P24" s="81"/>
       <c r="Q24" s="97"/>
       <c r="R24" s="48"/>
-      <c r="S24" s="166" t="s">
-        <v>506</v>
-      </c>
+      <c r="S24" s="166"/>
       <c r="T24" s="120" t="s">
         <v>97</v>
       </c>
@@ -23643,7 +23619,7 @@
         <v>620</v>
       </c>
       <c r="D25" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E25" s="77" t="s">
         <v>673</v>
@@ -23652,7 +23628,7 @@
         <v>487</v>
       </c>
       <c r="G25" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H25" s="79" t="s">
         <v>76</v>
@@ -23679,9 +23655,7 @@
       <c r="P25" s="81"/>
       <c r="Q25" s="97"/>
       <c r="R25" s="48"/>
-      <c r="S25" s="166" t="s">
-        <v>507</v>
-      </c>
+      <c r="S25" s="166"/>
       <c r="T25" s="120" t="s">
         <v>97</v>
       </c>
@@ -24705,7 +24679,7 @@
         <v>620</v>
       </c>
       <c r="D26" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E26" s="77" t="s">
         <v>674</v>
@@ -24714,7 +24688,7 @@
         <v>488</v>
       </c>
       <c r="G26" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H26" s="79" t="s">
         <v>76</v>
@@ -24741,9 +24715,7 @@
       <c r="P26" s="81"/>
       <c r="Q26" s="97"/>
       <c r="R26" s="48"/>
-      <c r="S26" s="163" t="s">
-        <v>133</v>
-      </c>
+      <c r="S26" s="163"/>
       <c r="T26" s="120" t="s">
         <v>97</v>
       </c>
@@ -25767,7 +25739,7 @@
         <v>620</v>
       </c>
       <c r="D27" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E27" s="77" t="s">
         <v>675</v>
@@ -25776,7 +25748,7 @@
         <v>134</v>
       </c>
       <c r="G27" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H27" s="79" t="s">
         <v>76</v>
@@ -25803,9 +25775,7 @@
       <c r="P27" s="81"/>
       <c r="Q27" s="97"/>
       <c r="R27" s="48"/>
-      <c r="S27" s="163" t="s">
-        <v>138</v>
-      </c>
+      <c r="S27" s="163"/>
       <c r="T27" s="120" t="s">
         <v>97</v>
       </c>
@@ -25839,7 +25809,7 @@
         <v>620</v>
       </c>
       <c r="D28" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E28" s="77" t="s">
         <v>676</v>
@@ -25848,7 +25818,7 @@
         <v>139</v>
       </c>
       <c r="G28" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H28" s="79" t="s">
         <v>76</v>
@@ -25875,9 +25845,7 @@
       <c r="P28" s="81"/>
       <c r="Q28" s="97"/>
       <c r="R28" s="48"/>
-      <c r="S28" s="163" t="s">
-        <v>143</v>
-      </c>
+      <c r="S28" s="163"/>
       <c r="T28" s="120" t="s">
         <v>97</v>
       </c>
@@ -26901,7 +26869,7 @@
         <v>620</v>
       </c>
       <c r="D29" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E29" s="77" t="s">
         <v>677</v>
@@ -26910,7 +26878,7 @@
         <v>144</v>
       </c>
       <c r="G29" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H29" s="79" t="s">
         <v>76</v>
@@ -26937,9 +26905,7 @@
       <c r="P29" s="81"/>
       <c r="Q29" s="97"/>
       <c r="R29" s="48"/>
-      <c r="S29" s="163" t="s">
-        <v>148</v>
-      </c>
+      <c r="S29" s="163"/>
       <c r="T29" s="120" t="s">
         <v>97</v>
       </c>
@@ -27963,7 +27929,7 @@
         <v>620</v>
       </c>
       <c r="D30" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E30" s="77" t="s">
         <v>678</v>
@@ -27972,7 +27938,7 @@
         <v>149</v>
       </c>
       <c r="G30" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H30" s="79" t="s">
         <v>76</v>
@@ -27999,9 +27965,7 @@
       <c r="P30" s="81"/>
       <c r="Q30" s="97"/>
       <c r="R30" s="48"/>
-      <c r="S30" s="163" t="s">
-        <v>153</v>
-      </c>
+      <c r="S30" s="163"/>
       <c r="T30" s="120" t="s">
         <v>97</v>
       </c>
@@ -29025,7 +28989,7 @@
         <v>620</v>
       </c>
       <c r="D31" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E31" s="77" t="s">
         <v>679</v>
@@ -29034,7 +28998,7 @@
         <v>154</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H31" s="79" t="s">
         <v>76</v>
@@ -29061,9 +29025,7 @@
       <c r="P31" s="81"/>
       <c r="Q31" s="97"/>
       <c r="R31" s="48"/>
-      <c r="S31" s="163" t="s">
-        <v>158</v>
-      </c>
+      <c r="S31" s="163"/>
       <c r="T31" s="120" t="s">
         <v>97</v>
       </c>
@@ -30087,7 +30049,7 @@
         <v>620</v>
       </c>
       <c r="D32" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E32" s="77" t="s">
         <v>680</v>
@@ -30096,7 +30058,7 @@
         <v>159</v>
       </c>
       <c r="G32" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H32" s="79" t="s">
         <v>76</v>
@@ -30123,9 +30085,7 @@
       <c r="P32" s="81"/>
       <c r="Q32" s="97"/>
       <c r="R32" s="48"/>
-      <c r="S32" s="163" t="s">
-        <v>162</v>
-      </c>
+      <c r="S32" s="163"/>
       <c r="T32" s="120" t="s">
         <v>97</v>
       </c>
@@ -31149,7 +31109,7 @@
         <v>620</v>
       </c>
       <c r="D33" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E33" s="77" t="s">
         <v>681</v>
@@ -31158,7 +31118,7 @@
         <v>163</v>
       </c>
       <c r="G33" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H33" s="79" t="s">
         <v>76</v>
@@ -31185,9 +31145,7 @@
       <c r="P33" s="81"/>
       <c r="Q33" s="97"/>
       <c r="R33" s="48"/>
-      <c r="S33" s="163" t="s">
-        <v>166</v>
-      </c>
+      <c r="S33" s="163"/>
       <c r="T33" s="120" t="s">
         <v>97</v>
       </c>
@@ -32211,7 +32169,7 @@
         <v>620</v>
       </c>
       <c r="D34" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E34" s="77" t="s">
         <v>682</v>
@@ -32220,7 +32178,7 @@
         <v>173</v>
       </c>
       <c r="G34" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H34" s="79" t="s">
         <v>76</v>
@@ -32247,9 +32205,7 @@
       <c r="P34" s="81"/>
       <c r="Q34" s="97"/>
       <c r="R34" s="48"/>
-      <c r="S34" s="163" t="s">
-        <v>169</v>
-      </c>
+      <c r="S34" s="163"/>
       <c r="T34" s="120" t="s">
         <v>97</v>
       </c>
@@ -33273,7 +33229,7 @@
         <v>620</v>
       </c>
       <c r="D35" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E35" s="77" t="s">
         <v>683</v>
@@ -33282,7 +33238,7 @@
         <v>177</v>
       </c>
       <c r="G35" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H35" s="79" t="s">
         <v>76</v>
@@ -33309,9 +33265,7 @@
       <c r="P35" s="81"/>
       <c r="Q35" s="97"/>
       <c r="R35" s="48"/>
-      <c r="S35" s="163" t="s">
-        <v>172</v>
-      </c>
+      <c r="S35" s="163"/>
       <c r="T35" s="120" t="s">
         <v>97</v>
       </c>
@@ -34335,7 +34289,7 @@
         <v>620</v>
       </c>
       <c r="D36" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E36" s="77" t="s">
         <v>684</v>
@@ -34344,7 +34298,7 @@
         <v>181</v>
       </c>
       <c r="G36" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H36" s="79" t="s">
         <v>76</v>
@@ -34371,9 +34325,7 @@
       <c r="P36" s="81"/>
       <c r="Q36" s="97"/>
       <c r="R36" s="48"/>
-      <c r="S36" s="163" t="s">
-        <v>176</v>
-      </c>
+      <c r="S36" s="163"/>
       <c r="T36" s="120" t="s">
         <v>97</v>
       </c>
@@ -34407,7 +34359,7 @@
         <v>620</v>
       </c>
       <c r="D37" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E37" s="77" t="s">
         <v>685</v>
@@ -34416,7 +34368,7 @@
         <v>185</v>
       </c>
       <c r="G37" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H37" s="79" t="s">
         <v>76</v>
@@ -34443,9 +34395,7 @@
       <c r="P37" s="81"/>
       <c r="Q37" s="97"/>
       <c r="R37" s="48"/>
-      <c r="S37" s="163" t="s">
-        <v>180</v>
-      </c>
+      <c r="S37" s="163"/>
       <c r="T37" s="120" t="s">
         <v>97</v>
       </c>
@@ -34479,7 +34429,7 @@
         <v>620</v>
       </c>
       <c r="D38" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E38" s="77" t="s">
         <v>686</v>
@@ -34488,7 +34438,7 @@
         <v>193</v>
       </c>
       <c r="G38" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H38" s="79" t="s">
         <v>76</v>
@@ -34515,9 +34465,7 @@
       <c r="P38" s="81"/>
       <c r="Q38" s="97"/>
       <c r="R38" s="48"/>
-      <c r="S38" s="163" t="s">
-        <v>184</v>
-      </c>
+      <c r="S38" s="163"/>
       <c r="T38" s="120" t="s">
         <v>97</v>
       </c>
@@ -34553,7 +34501,7 @@
         <v>620</v>
       </c>
       <c r="D39" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E39" s="77" t="s">
         <v>687</v>
@@ -34562,7 +34510,7 @@
         <v>197</v>
       </c>
       <c r="G39" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H39" s="79" t="s">
         <v>76</v>
@@ -34589,9 +34537,7 @@
       <c r="P39" s="81"/>
       <c r="Q39" s="97"/>
       <c r="R39" s="48"/>
-      <c r="S39" s="163" t="s">
-        <v>188</v>
-      </c>
+      <c r="S39" s="163"/>
       <c r="T39" s="120" t="s">
         <v>97</v>
       </c>
@@ -35617,7 +35563,7 @@
         <v>620</v>
       </c>
       <c r="D40" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E40" s="77" t="s">
         <v>688</v>
@@ -35626,7 +35572,7 @@
         <v>201</v>
       </c>
       <c r="G40" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H40" s="79" t="s">
         <v>76</v>
@@ -35653,9 +35599,7 @@
       <c r="P40" s="81"/>
       <c r="Q40" s="97"/>
       <c r="R40" s="48"/>
-      <c r="S40" s="164" t="s">
-        <v>494</v>
-      </c>
+      <c r="S40" s="164"/>
       <c r="T40" s="120" t="s">
         <v>97</v>
       </c>
@@ -36681,7 +36625,7 @@
         <v>620</v>
       </c>
       <c r="D41" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E41" s="77" t="s">
         <v>689</v>
@@ -36690,7 +36634,7 @@
         <v>204</v>
       </c>
       <c r="G41" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H41" s="79" t="s">
         <v>76</v>
@@ -36717,9 +36661,7 @@
       <c r="P41" s="81"/>
       <c r="Q41" s="97"/>
       <c r="R41" s="48"/>
-      <c r="S41" s="163" t="s">
-        <v>192</v>
-      </c>
+      <c r="S41" s="163"/>
       <c r="T41" s="120" t="s">
         <v>97</v>
       </c>
@@ -37745,7 +37687,7 @@
         <v>620</v>
       </c>
       <c r="D42" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E42" s="77" t="s">
         <v>690</v>
@@ -37754,7 +37696,7 @@
         <v>208</v>
       </c>
       <c r="G42" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H42" s="79" t="s">
         <v>76</v>
@@ -37781,9 +37723,7 @@
       <c r="P42" s="81"/>
       <c r="Q42" s="97"/>
       <c r="R42" s="48"/>
-      <c r="S42" s="163" t="s">
-        <v>196</v>
-      </c>
+      <c r="S42" s="163"/>
       <c r="T42" s="120" t="s">
         <v>97</v>
       </c>
@@ -38809,7 +38749,7 @@
         <v>620</v>
       </c>
       <c r="D43" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E43" s="77" t="s">
         <v>691</v>
@@ -38818,7 +38758,7 @@
         <v>518</v>
       </c>
       <c r="G43" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H43" s="79" t="s">
         <v>76</v>
@@ -38845,9 +38785,7 @@
       <c r="P43" s="81"/>
       <c r="Q43" s="97"/>
       <c r="R43" s="48"/>
-      <c r="S43" s="163" t="s">
-        <v>200</v>
-      </c>
+      <c r="S43" s="163"/>
       <c r="T43" s="120" t="s">
         <v>97</v>
       </c>
@@ -39873,7 +39811,7 @@
         <v>620</v>
       </c>
       <c r="D44" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E44" s="77" t="s">
         <v>692</v>
@@ -39882,7 +39820,7 @@
         <v>530</v>
       </c>
       <c r="G44" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H44" s="79" t="s">
         <v>76</v>
@@ -39909,9 +39847,7 @@
       <c r="P44" s="81"/>
       <c r="Q44" s="97"/>
       <c r="R44" s="48"/>
-      <c r="S44" s="163" t="s">
-        <v>207</v>
-      </c>
+      <c r="S44" s="163"/>
       <c r="T44" s="120" t="s">
         <v>97</v>
       </c>
@@ -40937,7 +40873,7 @@
         <v>620</v>
       </c>
       <c r="D45" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E45" s="77" t="s">
         <v>693</v>
@@ -40946,7 +40882,7 @@
         <v>212</v>
       </c>
       <c r="G45" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H45" s="79" t="s">
         <v>76</v>
@@ -40973,9 +40909,7 @@
       <c r="P45" s="81"/>
       <c r="Q45" s="97"/>
       <c r="R45" s="48"/>
-      <c r="S45" s="163" t="s">
-        <v>211</v>
-      </c>
+      <c r="S45" s="163"/>
       <c r="T45" s="120" t="s">
         <v>97</v>
       </c>
@@ -42001,7 +41935,7 @@
         <v>620</v>
       </c>
       <c r="D46" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E46" s="77" t="s">
         <v>694</v>
@@ -42010,7 +41944,7 @@
         <v>216</v>
       </c>
       <c r="G46" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H46" s="79" t="s">
         <v>76</v>
@@ -42037,9 +41971,7 @@
       <c r="P46" s="81"/>
       <c r="Q46" s="97"/>
       <c r="R46" s="48"/>
-      <c r="S46" s="163" t="s">
-        <v>215</v>
-      </c>
+      <c r="S46" s="163"/>
       <c r="T46" s="120" t="s">
         <v>97</v>
       </c>
@@ -43065,7 +42997,7 @@
         <v>620</v>
       </c>
       <c r="D47" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E47" s="77" t="s">
         <v>695</v>
@@ -43074,7 +43006,7 @@
         <v>220</v>
       </c>
       <c r="G47" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H47" s="79" t="s">
         <v>76</v>
@@ -43101,9 +43033,7 @@
       <c r="P47" s="81"/>
       <c r="Q47" s="97"/>
       <c r="R47" s="48"/>
-      <c r="S47" s="163" t="s">
-        <v>219</v>
-      </c>
+      <c r="S47" s="163"/>
       <c r="T47" s="120" t="s">
         <v>97</v>
       </c>
@@ -44129,7 +44059,7 @@
         <v>620</v>
       </c>
       <c r="D48" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E48" s="77" t="s">
         <v>696</v>
@@ -44138,7 +44068,7 @@
         <v>224</v>
       </c>
       <c r="G48" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H48" s="79" t="s">
         <v>76</v>
@@ -44165,9 +44095,7 @@
       <c r="P48" s="81"/>
       <c r="Q48" s="97"/>
       <c r="R48" s="48"/>
-      <c r="S48" s="163" t="s">
-        <v>223</v>
-      </c>
+      <c r="S48" s="163"/>
       <c r="T48" s="120" t="s">
         <v>97</v>
       </c>
@@ -45193,7 +45121,7 @@
         <v>620</v>
       </c>
       <c r="D49" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E49" s="77" t="s">
         <v>697</v>
@@ -45202,7 +45130,7 @@
         <v>228</v>
       </c>
       <c r="G49" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H49" s="79" t="s">
         <v>76</v>
@@ -45229,9 +45157,7 @@
       <c r="P49" s="81"/>
       <c r="Q49" s="97"/>
       <c r="R49" s="48"/>
-      <c r="S49" s="163" t="s">
-        <v>227</v>
-      </c>
+      <c r="S49" s="163"/>
       <c r="T49" s="120" t="s">
         <v>97</v>
       </c>
@@ -46257,7 +46183,7 @@
         <v>620</v>
       </c>
       <c r="D50" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E50" s="77" t="s">
         <v>698</v>
@@ -46266,7 +46192,7 @@
         <v>517</v>
       </c>
       <c r="G50" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H50" s="79" t="s">
         <v>76</v>
@@ -46293,9 +46219,7 @@
       <c r="P50" s="81"/>
       <c r="Q50" s="97"/>
       <c r="R50" s="48"/>
-      <c r="S50" s="163" t="s">
-        <v>231</v>
-      </c>
+      <c r="S50" s="163"/>
       <c r="T50" s="120" t="s">
         <v>97</v>
       </c>
@@ -46331,7 +46255,7 @@
         <v>620</v>
       </c>
       <c r="D51" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E51" s="77" t="s">
         <v>699</v>
@@ -46340,7 +46264,7 @@
         <v>573</v>
       </c>
       <c r="G51" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H51" s="79" t="s">
         <v>76</v>
@@ -46367,9 +46291,7 @@
       <c r="P51" s="81"/>
       <c r="Q51" s="97"/>
       <c r="R51" s="48"/>
-      <c r="S51" s="163" t="s">
-        <v>235</v>
-      </c>
+      <c r="S51" s="163"/>
       <c r="T51" s="120" t="s">
         <v>97</v>
       </c>
@@ -47395,7 +47317,7 @@
         <v>620</v>
       </c>
       <c r="D52" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E52" s="77" t="s">
         <v>700</v>
@@ -47404,7 +47326,7 @@
         <v>573</v>
       </c>
       <c r="G52" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H52" s="79" t="s">
         <v>76</v>
@@ -47431,9 +47353,7 @@
       <c r="P52" s="81"/>
       <c r="Q52" s="97"/>
       <c r="R52" s="48"/>
-      <c r="S52" s="164" t="s">
-        <v>510</v>
-      </c>
+      <c r="S52" s="164"/>
       <c r="T52" s="120" t="s">
         <v>97</v>
       </c>
@@ -48459,7 +48379,7 @@
         <v>620</v>
       </c>
       <c r="D53" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E53" s="77" t="s">
         <v>701</v>
@@ -48468,7 +48388,7 @@
         <v>573</v>
       </c>
       <c r="G53" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H53" s="79" t="s">
         <v>76</v>
@@ -48495,9 +48415,7 @@
       <c r="P53" s="81"/>
       <c r="Q53" s="97"/>
       <c r="R53" s="48"/>
-      <c r="S53" s="163" t="s">
-        <v>238</v>
-      </c>
+      <c r="S53" s="163"/>
       <c r="T53" s="120" t="s">
         <v>97</v>
       </c>
@@ -49523,7 +49441,7 @@
         <v>620</v>
       </c>
       <c r="D54" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E54" s="77" t="s">
         <v>702</v>
@@ -49532,7 +49450,7 @@
         <v>573</v>
       </c>
       <c r="G54" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H54" s="79" t="s">
         <v>76</v>
@@ -49559,9 +49477,7 @@
       <c r="P54" s="81"/>
       <c r="Q54" s="97"/>
       <c r="R54" s="48"/>
-      <c r="S54" s="163" t="s">
-        <v>242</v>
-      </c>
+      <c r="S54" s="163"/>
       <c r="T54" s="120" t="s">
         <v>97</v>
       </c>
@@ -50587,7 +50503,7 @@
         <v>620</v>
       </c>
       <c r="D55" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E55" s="77" t="s">
         <v>703</v>
@@ -50596,7 +50512,7 @@
         <v>573</v>
       </c>
       <c r="G55" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H55" s="79" t="s">
         <v>76</v>
@@ -50623,9 +50539,7 @@
       <c r="P55" s="81"/>
       <c r="Q55" s="97"/>
       <c r="R55" s="48"/>
-      <c r="S55" s="164" t="s">
-        <v>246</v>
-      </c>
+      <c r="S55" s="164"/>
       <c r="T55" s="120" t="s">
         <v>97</v>
       </c>
@@ -51651,7 +51565,7 @@
         <v>620</v>
       </c>
       <c r="D56" s="77" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="E56" s="77" t="s">
         <v>704</v>
@@ -51660,7 +51574,7 @@
         <v>573</v>
       </c>
       <c r="G56" s="78" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="H56" s="79" t="s">
         <v>76</v>
@@ -51687,9 +51601,7 @@
       <c r="P56" s="81"/>
       <c r="Q56" s="97"/>
       <c r="R56" s="48"/>
-      <c r="S56" s="167" t="s">
-        <v>249</v>
-      </c>
+      <c r="S56" s="167"/>
       <c r="T56" s="120" t="s">
         <v>97</v>
       </c>

</xml_diff>